<commit_message>
HoldProcess migrated to 1.1.0 version of SharedContext
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\HoldProcess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC14D9A-96A2-496C-9F56-A57F6CE332A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A87C66C-FD07-4E8C-94EE-F94ADECED84B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31335" yWindow="2850" windowWidth="20355" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5355" yWindow="3675" windowWidth="20100" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConfigDict" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,6 @@
     <t>Message2nd</t>
   </si>
   <si>
-    <t>El cliente ha estado X segundos en Hold, por favor retoma la llamada cuanto antes</t>
-  </si>
-  <si>
-    <t>El cliente ha estado Y segundos en Hold. Cuando aceptes este mensaje la llamada se retomara.</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
@@ -49,6 +43,12 @@
   </si>
   <si>
     <t>WaitingTime2nd</t>
+  </si>
+  <si>
+    <t>El cliente ha estado 5 segundos en Hold, por favor retoma la llamada cuanto antes</t>
+  </si>
+  <si>
+    <t>El cliente ha estado 10 segundos en Hold. Cuando aceptes este mensaje la llamada se retomara.</t>
   </si>
 </sst>
 </file>
@@ -379,7 +379,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,10 +390,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -409,12 +409,12 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -425,7 +425,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>